<commit_message>
Other ATTCK module updated
</commit_message>
<xml_diff>
--- a/attck_windows_tech.xlsx
+++ b/attck_windows_tech.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5460" yWindow="-120" windowWidth="15630" windowHeight="7395"/>
+    <workbookView xWindow="6390" yWindow="-120" windowWidth="15630" windowHeight="7395"/>
   </bookViews>
   <sheets>
     <sheet name="To do" sheetId="3" r:id="rId1"/>
@@ -889,7 +889,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -916,6 +916,14 @@
       <b/>
       <sz val="14"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -977,7 +985,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1043,9 +1051,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1202,12 +1211,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1217,18 +1220,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1263,16 +1254,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1312,193 +1293,222 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1814,9 +1824,9 @@
   <dimension ref="A1:XFD83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1:F1"/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1840,438 +1850,438 @@
       <c r="C1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="109" t="s">
+      <c r="D1" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="109"/>
-      <c r="F1" s="109"/>
-    </row>
-    <row r="2" spans="1:6 16384:16384" s="87" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="84">
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+    </row>
+    <row r="2" spans="1:6 16384:16384" s="77" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="153">
         <v>1</v>
       </c>
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="97" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="85" t="s">
+      <c r="C2" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="84" t="s">
+      <c r="D2" s="74" t="s">
         <v>218</v>
       </c>
-      <c r="E2" s="84"/>
-      <c r="F2" s="86" t="s">
+      <c r="E2" s="74"/>
+      <c r="F2" s="76" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="3" spans="1:6 16384:16384" s="69" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="64"/>
-      <c r="B3" s="113"/>
-      <c r="C3" s="65" t="s">
+    <row r="3" spans="1:6 16384:16384" s="63" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="154"/>
+      <c r="B3" s="98"/>
+      <c r="C3" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66" t="s">
+      <c r="D3" s="60"/>
+      <c r="E3" s="157" t="s">
         <v>267</v>
       </c>
-      <c r="F3" s="67" t="s">
+      <c r="F3" s="61" t="s">
         <v>266</v>
       </c>
-      <c r="XFD3" s="68" t="s">
+      <c r="XFD3" s="62" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="4" spans="1:6 16384:16384" s="80" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="112">
+    <row r="4" spans="1:6 16384:16384" s="136" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="97">
         <v>2</v>
       </c>
-      <c r="B4" s="112" t="s">
+      <c r="B4" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="77" t="s">
+      <c r="C4" s="133" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="78" t="s">
+      <c r="D4" s="134" t="s">
         <v>220</v>
       </c>
-      <c r="E4" s="78"/>
-      <c r="F4" s="79" t="s">
+      <c r="E4" s="134"/>
+      <c r="F4" s="135" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="5" spans="1:6 16384:16384" s="76" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="113"/>
-      <c r="B5" s="113"/>
-      <c r="C5" s="74" t="s">
+    <row r="5" spans="1:6 16384:16384" s="70" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="98"/>
+      <c r="B5" s="98"/>
+      <c r="C5" s="68" t="s">
         <v>221</v>
       </c>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="67" t="s">
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="61" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="6" spans="1:6 16384:16384" s="73" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="106">
+    <row r="6" spans="1:6 16384:16384" s="67" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="93">
         <v>3</v>
       </c>
-      <c r="B6" s="106" t="s">
+      <c r="B6" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="70" t="s">
+      <c r="C6" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="72" t="s">
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="66" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="7" spans="1:6 16384:16384" s="83" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="107"/>
-      <c r="B7" s="107"/>
-      <c r="C7" s="103" t="s">
+    <row r="7" spans="1:6 16384:16384" s="73" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="94"/>
+      <c r="B7" s="94"/>
+      <c r="C7" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="81" t="s">
+      <c r="D7" s="71" t="s">
         <v>222</v>
       </c>
-      <c r="E7" s="81"/>
-      <c r="F7" s="82" t="s">
+      <c r="E7" s="71"/>
+      <c r="F7" s="72" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="8" spans="1:6 16384:16384" s="83" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="107"/>
-      <c r="B8" s="107"/>
-      <c r="C8" s="104"/>
-      <c r="D8" s="81" t="s">
+    <row r="8" spans="1:6 16384:16384" s="73" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="94"/>
+      <c r="B8" s="94"/>
+      <c r="C8" s="89"/>
+      <c r="D8" s="71" t="s">
         <v>56</v>
       </c>
-      <c r="E8" s="81"/>
-      <c r="F8" s="82" t="s">
+      <c r="E8" s="71"/>
+      <c r="F8" s="72" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="9" spans="1:6 16384:16384" s="83" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="107"/>
-      <c r="B9" s="107"/>
-      <c r="C9" s="103" t="s">
+    <row r="9" spans="1:6 16384:16384" s="73" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="94"/>
+      <c r="B9" s="94"/>
+      <c r="C9" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="81" t="s">
+      <c r="D9" s="71" t="s">
         <v>61</v>
       </c>
-      <c r="E9" s="81"/>
-      <c r="F9" s="82" t="s">
+      <c r="E9" s="71"/>
+      <c r="F9" s="72" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="10" spans="1:6 16384:16384" s="83" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="107"/>
-      <c r="B10" s="107"/>
-      <c r="C10" s="105"/>
-      <c r="D10" s="84" t="s">
+    <row r="10" spans="1:6 16384:16384" s="73" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="94"/>
+      <c r="B10" s="94"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="74" t="s">
         <v>223</v>
       </c>
-      <c r="E10" s="84"/>
-      <c r="F10" s="88" t="s">
+      <c r="E10" s="74"/>
+      <c r="F10" s="78" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="11" spans="1:6 16384:16384" s="83" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="107"/>
-      <c r="B11" s="107"/>
-      <c r="C11" s="105"/>
-      <c r="D11" s="84" t="s">
+    <row r="11" spans="1:6 16384:16384" s="73" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="94"/>
+      <c r="B11" s="94"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="74" t="s">
         <v>224</v>
       </c>
-      <c r="E11" s="84"/>
-      <c r="F11" s="88" t="s">
+      <c r="E11" s="74"/>
+      <c r="F11" s="78" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="12" spans="1:6 16384:16384" s="83" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="107"/>
-      <c r="B12" s="107"/>
-      <c r="C12" s="105"/>
-      <c r="D12" s="84" t="s">
+    <row r="12" spans="1:6 16384:16384" s="73" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="94"/>
+      <c r="B12" s="94"/>
+      <c r="C12" s="88"/>
+      <c r="D12" s="74" t="s">
         <v>226</v>
       </c>
-      <c r="E12" s="84"/>
-      <c r="F12" s="88" t="s">
+      <c r="E12" s="74"/>
+      <c r="F12" s="78" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="13" spans="1:6 16384:16384" s="83" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="107"/>
-      <c r="B13" s="107"/>
-      <c r="C13" s="104"/>
-      <c r="D13" s="84" t="s">
+    <row r="13" spans="1:6 16384:16384" s="73" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="94"/>
+      <c r="B13" s="94"/>
+      <c r="C13" s="89"/>
+      <c r="D13" s="74" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="84"/>
-      <c r="F13" s="88" t="s">
+      <c r="E13" s="74"/>
+      <c r="F13" s="78" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="14" spans="1:6 16384:16384" s="91" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="107"/>
-      <c r="B14" s="107"/>
-      <c r="C14" s="93" t="s">
+    <row r="14" spans="1:6 16384:16384" s="81" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="94"/>
+      <c r="B14" s="94"/>
+      <c r="C14" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="66"/>
-      <c r="E14" s="66" t="s">
+      <c r="D14" s="60"/>
+      <c r="E14" s="60" t="s">
         <v>273</v>
       </c>
-      <c r="F14" s="90" t="s">
+      <c r="F14" s="80" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="15" spans="1:6 16384:16384" s="83" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="107"/>
-      <c r="B15" s="107"/>
-      <c r="C15" s="103" t="s">
+    <row r="15" spans="1:6 16384:16384" s="73" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="94"/>
+      <c r="B15" s="94"/>
+      <c r="C15" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="84" t="s">
+      <c r="D15" s="74" t="s">
         <v>228</v>
       </c>
-      <c r="E15" s="84"/>
-      <c r="F15" s="88" t="s">
+      <c r="E15" s="74"/>
+      <c r="F15" s="78" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="16" spans="1:6 16384:16384" s="83" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="107"/>
-      <c r="B16" s="107"/>
-      <c r="C16" s="105"/>
-      <c r="D16" s="84" t="s">
+    <row r="16" spans="1:6 16384:16384" s="73" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="94"/>
+      <c r="B16" s="94"/>
+      <c r="C16" s="88"/>
+      <c r="D16" s="74" t="s">
         <v>230</v>
       </c>
-      <c r="E16" s="84"/>
-      <c r="F16" s="88" t="s">
+      <c r="E16" s="74"/>
+      <c r="F16" s="78" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="91" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="107"/>
-      <c r="B17" s="107"/>
-      <c r="C17" s="104"/>
-      <c r="D17" s="66" t="s">
+    <row r="17" spans="1:6" s="81" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="94"/>
+      <c r="B17" s="94"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="60" t="s">
         <v>232</v>
       </c>
-      <c r="E17" s="66"/>
-      <c r="F17" s="90" t="s">
+      <c r="E17" s="60"/>
+      <c r="F17" s="80" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="83" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="107"/>
-      <c r="B18" s="107"/>
-      <c r="C18" s="89" t="s">
+    <row r="18" spans="1:6" s="73" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="94"/>
+      <c r="B18" s="94"/>
+      <c r="C18" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="84" t="s">
+      <c r="D18" s="74" t="s">
         <v>233</v>
       </c>
-      <c r="E18" s="84"/>
-      <c r="F18" s="88" t="s">
+      <c r="E18" s="74"/>
+      <c r="F18" s="78" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="91" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="107"/>
-      <c r="B19" s="107"/>
-      <c r="C19" s="92" t="s">
+    <row r="19" spans="1:6" s="81" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="94"/>
+      <c r="B19" s="94"/>
+      <c r="C19" s="82" t="s">
         <v>75</v>
       </c>
-      <c r="D19" s="66"/>
-      <c r="E19" s="66"/>
-      <c r="F19" s="90" t="s">
+      <c r="D19" s="60"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="80" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="107"/>
-      <c r="B20" s="107"/>
-      <c r="C20" s="56" t="s">
+    <row r="20" spans="1:6" s="140" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="94"/>
+      <c r="B20" s="94"/>
+      <c r="C20" s="137" t="s">
         <v>78</v>
       </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6" t="s">
+      <c r="D20" s="138"/>
+      <c r="E20" s="138" t="s">
         <v>263</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="139" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="83" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="107"/>
-      <c r="B21" s="107"/>
-      <c r="C21" s="100" t="s">
+    <row r="21" spans="1:6" s="73" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="94"/>
+      <c r="B21" s="94"/>
+      <c r="C21" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="84" t="s">
+      <c r="D21" s="74" t="s">
         <v>235</v>
       </c>
-      <c r="E21" s="84"/>
-      <c r="F21" s="88" t="s">
+      <c r="E21" s="74"/>
+      <c r="F21" s="78" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="98" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="107"/>
-      <c r="B22" s="107"/>
-      <c r="C22" s="114" t="s">
+    <row r="22" spans="1:6" s="140" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="94"/>
+      <c r="B22" s="94"/>
+      <c r="C22" s="141" t="s">
         <v>237</v>
       </c>
-      <c r="D22" s="96" t="s">
+      <c r="D22" s="138" t="s">
         <v>238</v>
       </c>
-      <c r="E22" s="97"/>
-      <c r="F22" s="110" t="s">
+      <c r="E22" s="142"/>
+      <c r="F22" s="143" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="98" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="107"/>
-      <c r="B23" s="107"/>
-      <c r="C23" s="115"/>
-      <c r="D23" s="96" t="s">
+    <row r="23" spans="1:6" s="140" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="94"/>
+      <c r="B23" s="94"/>
+      <c r="C23" s="144"/>
+      <c r="D23" s="138" t="s">
         <v>240</v>
       </c>
-      <c r="E23" s="99"/>
-      <c r="F23" s="111"/>
-    </row>
-    <row r="24" spans="1:6" s="91" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="108"/>
-      <c r="B24" s="108"/>
-      <c r="C24" s="93" t="s">
+      <c r="E23" s="145"/>
+      <c r="F23" s="146"/>
+    </row>
+    <row r="24" spans="1:6" s="81" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="95"/>
+      <c r="B24" s="95"/>
+      <c r="C24" s="83" t="s">
         <v>94</v>
       </c>
-      <c r="D24" s="66"/>
-      <c r="E24" s="94" t="s">
+      <c r="D24" s="60"/>
+      <c r="E24" s="84" t="s">
         <v>265</v>
       </c>
-      <c r="F24" s="95" t="s">
+      <c r="F24" s="85" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="83" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="116">
+    <row r="25" spans="1:6" s="140" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="151">
         <v>4</v>
       </c>
-      <c r="B25" s="116" t="s">
+      <c r="B25" s="151" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="103" t="s">
+      <c r="C25" s="141" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="84" t="s">
+      <c r="D25" s="138" t="s">
         <v>241</v>
       </c>
-      <c r="E25" s="101"/>
-      <c r="F25" s="119" t="s">
+      <c r="E25" s="142"/>
+      <c r="F25" s="143" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="83" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="116"/>
-      <c r="B26" s="116"/>
-      <c r="C26" s="105"/>
-      <c r="D26" s="84" t="s">
+    <row r="26" spans="1:6" s="140" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="151"/>
+      <c r="B26" s="151"/>
+      <c r="C26" s="147"/>
+      <c r="D26" s="138" t="s">
         <v>243</v>
       </c>
-      <c r="E26" s="81"/>
-      <c r="F26" s="120"/>
-    </row>
-    <row r="27" spans="1:6" s="83" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="116"/>
-      <c r="B27" s="116"/>
-      <c r="C27" s="104"/>
-      <c r="D27" s="84" t="s">
+      <c r="E26" s="145"/>
+      <c r="F26" s="146"/>
+    </row>
+    <row r="27" spans="1:6" s="140" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="151"/>
+      <c r="B27" s="151"/>
+      <c r="C27" s="144"/>
+      <c r="D27" s="138" t="s">
         <v>244</v>
       </c>
-      <c r="E27" s="84"/>
-      <c r="F27" s="102" t="s">
+      <c r="E27" s="138"/>
+      <c r="F27" s="152" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="116"/>
-      <c r="B28" s="116"/>
-      <c r="C28" s="121" t="s">
+    <row r="28" spans="1:6" s="140" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="151"/>
+      <c r="B28" s="151"/>
+      <c r="C28" s="141" t="s">
         <v>246</v>
       </c>
-      <c r="D28" s="46" t="s">
+      <c r="D28" s="138" t="s">
         <v>247</v>
       </c>
-      <c r="E28" s="57"/>
-      <c r="F28" s="117" t="s">
+      <c r="E28" s="142"/>
+      <c r="F28" s="143" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="116"/>
-      <c r="B29" s="116"/>
-      <c r="C29" s="122"/>
-      <c r="D29" s="30" t="s">
+    <row r="29" spans="1:6" s="140" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="151"/>
+      <c r="B29" s="151"/>
+      <c r="C29" s="147"/>
+      <c r="D29" s="134" t="s">
         <v>249</v>
       </c>
-      <c r="E29" s="62"/>
-      <c r="F29" s="118"/>
-    </row>
-    <row r="30" spans="1:6" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="116"/>
-      <c r="B30" s="116"/>
-      <c r="C30" s="122"/>
-      <c r="D30" s="30" t="s">
+      <c r="E29" s="148"/>
+      <c r="F29" s="146"/>
+    </row>
+    <row r="30" spans="1:6" s="140" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="151"/>
+      <c r="B30" s="151"/>
+      <c r="C30" s="147"/>
+      <c r="D30" s="134" t="s">
         <v>250</v>
       </c>
-      <c r="E30" s="63"/>
-      <c r="F30" s="117" t="s">
+      <c r="E30" s="149"/>
+      <c r="F30" s="143" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="116"/>
-      <c r="B31" s="116"/>
-      <c r="C31" s="123"/>
-      <c r="D31" s="30" t="s">
+    <row r="31" spans="1:6" s="140" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="151"/>
+      <c r="B31" s="151"/>
+      <c r="C31" s="144"/>
+      <c r="D31" s="134" t="s">
         <v>251</v>
       </c>
-      <c r="E31" s="62"/>
-      <c r="F31" s="118"/>
-    </row>
-    <row r="32" spans="1:6" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="34">
+      <c r="E31" s="148"/>
+      <c r="F31" s="146"/>
+    </row>
+    <row r="32" spans="1:6" s="140" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="134">
         <v>5</v>
       </c>
-      <c r="B32" s="34" t="s">
+      <c r="B32" s="134" t="s">
         <v>252</v>
       </c>
-      <c r="C32" s="26"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="50" t="s">
+      <c r="C32" s="150"/>
+      <c r="D32" s="134"/>
+      <c r="E32" s="134"/>
+      <c r="F32" s="139" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="34">
+    <row r="33" spans="1:6" s="81" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="69">
         <v>6</v>
       </c>
-      <c r="B33" s="34" t="s">
+      <c r="B33" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="61" t="s">
+      <c r="C33" s="155" t="s">
         <v>254</v>
       </c>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="27" t="s">
+      <c r="D33" s="69"/>
+      <c r="E33" s="69"/>
+      <c r="F33" s="156" t="s">
         <v>255</v>
       </c>
     </row>
@@ -2505,14 +2515,7 @@
     <row r="82" x14ac:dyDescent="0.25"/>
     <row r="83" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="B25:B31"/>
-    <mergeCell ref="A25:A31"/>
-    <mergeCell ref="C25:C27"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="C28:C31"/>
+  <mergeCells count="19">
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="C9:C13"/>
     <mergeCell ref="B6:B24"/>
@@ -2524,9 +2527,20 @@
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C22:C23"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B25:B31"/>
+    <mergeCell ref="A25:A31"/>
+    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="C28:C31"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2535,7 +2549,7 @@
   <dimension ref="A1:XFC162"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
     </sheetView>
@@ -2562,59 +2576,59 @@
       <c r="C1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="109" t="s">
+      <c r="D1" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="109"/>
+      <c r="E1" s="96"/>
     </row>
     <row r="2" spans="1:5" s="32" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="112">
+      <c r="A2" s="97">
         <v>1</v>
       </c>
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="97" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="138" t="s">
+      <c r="C2" s="116" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="142" t="s">
+      <c r="E2" s="110" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="32" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="137"/>
-      <c r="B3" s="137"/>
-      <c r="C3" s="148"/>
+      <c r="A3" s="119"/>
+      <c r="B3" s="119"/>
+      <c r="C3" s="117"/>
       <c r="D3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="143"/>
+      <c r="E3" s="111"/>
     </row>
     <row r="4" spans="1:5" s="32" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="137"/>
-      <c r="B4" s="137"/>
-      <c r="C4" s="148"/>
+      <c r="A4" s="119"/>
+      <c r="B4" s="119"/>
+      <c r="C4" s="117"/>
       <c r="D4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="143"/>
+      <c r="E4" s="111"/>
     </row>
     <row r="5" spans="1:5" s="32" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="137"/>
-      <c r="B5" s="137"/>
-      <c r="C5" s="139"/>
+      <c r="A5" s="119"/>
+      <c r="B5" s="119"/>
+      <c r="C5" s="118"/>
       <c r="D5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="144"/>
+      <c r="E5" s="112"/>
     </row>
     <row r="6" spans="1:5" s="32" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="137"/>
-      <c r="B6" s="137"/>
-      <c r="C6" s="138" t="s">
+      <c r="A6" s="119"/>
+      <c r="B6" s="119"/>
+      <c r="C6" s="116" t="s">
         <v>26</v>
       </c>
       <c r="D6" s="5" t="s">
@@ -2625,9 +2639,9 @@
       </c>
     </row>
     <row r="7" spans="1:5" s="32" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="137"/>
-      <c r="B7" s="137"/>
-      <c r="C7" s="139"/>
+      <c r="A7" s="119"/>
+      <c r="B7" s="119"/>
+      <c r="C7" s="118"/>
       <c r="D7" s="5" t="s">
         <v>38</v>
       </c>
@@ -2636,8 +2650,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" s="32" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="137"/>
-      <c r="B8" s="137"/>
+      <c r="A8" s="119"/>
+      <c r="B8" s="119"/>
       <c r="C8" s="37" t="s">
         <v>27</v>
       </c>
@@ -2647,8 +2661,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" s="32" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="137"/>
-      <c r="B9" s="137"/>
+      <c r="A9" s="119"/>
+      <c r="B9" s="119"/>
       <c r="C9" s="37" t="s">
         <v>31</v>
       </c>
@@ -2658,8 +2672,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" s="32" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="137"/>
-      <c r="B10" s="137"/>
+      <c r="A10" s="119"/>
+      <c r="B10" s="119"/>
       <c r="C10" s="37" t="s">
         <v>32</v>
       </c>
@@ -2669,8 +2683,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" s="32" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="137"/>
-      <c r="B11" s="137"/>
+      <c r="A11" s="119"/>
+      <c r="B11" s="119"/>
       <c r="C11" s="37" t="s">
         <v>34</v>
       </c>
@@ -2680,10 +2694,10 @@
       </c>
     </row>
     <row r="12" spans="1:5" s="32" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="112">
+      <c r="A12" s="97">
         <v>2</v>
       </c>
-      <c r="B12" s="112" t="s">
+      <c r="B12" s="97" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="37" t="s">
@@ -2697,48 +2711,48 @@
       </c>
     </row>
     <row r="13" spans="1:5" s="32" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="137"/>
-      <c r="B13" s="137"/>
-      <c r="C13" s="145" t="s">
+      <c r="A13" s="119"/>
+      <c r="B13" s="119"/>
+      <c r="C13" s="113" t="s">
         <v>20</v>
       </c>
       <c r="D13" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="142" t="s">
+      <c r="E13" s="110" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="32" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="137"/>
-      <c r="B14" s="137"/>
-      <c r="C14" s="146"/>
+      <c r="A14" s="119"/>
+      <c r="B14" s="119"/>
+      <c r="C14" s="114"/>
       <c r="D14" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="143"/>
+      <c r="E14" s="111"/>
     </row>
     <row r="15" spans="1:5" s="32" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="137"/>
-      <c r="B15" s="137"/>
-      <c r="C15" s="146"/>
+      <c r="A15" s="119"/>
+      <c r="B15" s="119"/>
+      <c r="C15" s="114"/>
       <c r="D15" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="143"/>
+      <c r="E15" s="111"/>
     </row>
     <row r="16" spans="1:5" s="26" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="137"/>
-      <c r="B16" s="137"/>
-      <c r="C16" s="147"/>
+      <c r="A16" s="119"/>
+      <c r="B16" s="119"/>
+      <c r="C16" s="115"/>
       <c r="D16" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="144"/>
+      <c r="E16" s="112"/>
     </row>
     <row r="17" spans="1:5" s="41" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="113"/>
-      <c r="B17" s="113"/>
+      <c r="A17" s="98"/>
+      <c r="B17" s="98"/>
       <c r="C17" s="39" t="s">
         <v>46</v>
       </c>
@@ -2748,10 +2762,10 @@
       </c>
     </row>
     <row r="18" spans="1:5" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="106">
+      <c r="A18" s="93">
         <v>3</v>
       </c>
-      <c r="B18" s="106" t="s">
+      <c r="B18" s="93" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="35" t="s">
@@ -2763,8 +2777,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="107"/>
-      <c r="B19" s="107"/>
+      <c r="A19" s="94"/>
+      <c r="B19" s="94"/>
       <c r="C19" s="35" t="s">
         <v>51</v>
       </c>
@@ -2774,8 +2788,8 @@
       </c>
     </row>
     <row r="20" spans="1:5" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="107"/>
-      <c r="B20" s="107"/>
+      <c r="A20" s="94"/>
+      <c r="B20" s="94"/>
       <c r="C20" s="7" t="s">
         <v>52</v>
       </c>
@@ -2787,9 +2801,9 @@
       </c>
     </row>
     <row r="21" spans="1:5" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="107"/>
-      <c r="B21" s="107"/>
-      <c r="C21" s="149"/>
+      <c r="A21" s="94"/>
+      <c r="B21" s="94"/>
+      <c r="C21" s="108"/>
       <c r="D21" s="16" t="s">
         <v>57</v>
       </c>
@@ -2798,9 +2812,9 @@
       </c>
     </row>
     <row r="22" spans="1:5" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="107"/>
-      <c r="B22" s="107"/>
-      <c r="C22" s="141"/>
+      <c r="A22" s="94"/>
+      <c r="B22" s="94"/>
+      <c r="C22" s="109"/>
       <c r="D22" s="16" t="s">
         <v>59</v>
       </c>
@@ -2809,9 +2823,9 @@
       </c>
     </row>
     <row r="23" spans="1:5" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="107"/>
-      <c r="B23" s="107"/>
-      <c r="C23" s="140" t="s">
+      <c r="A23" s="94"/>
+      <c r="B23" s="94"/>
+      <c r="C23" s="107" t="s">
         <v>8</v>
       </c>
       <c r="D23" s="6" t="s">
@@ -2822,9 +2836,9 @@
       </c>
     </row>
     <row r="24" spans="1:5" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="107"/>
-      <c r="B24" s="107"/>
-      <c r="C24" s="141"/>
+      <c r="A24" s="94"/>
+      <c r="B24" s="94"/>
+      <c r="C24" s="109"/>
       <c r="D24" s="6" t="s">
         <v>66</v>
       </c>
@@ -2833,50 +2847,50 @@
       </c>
     </row>
     <row r="25" spans="1:5" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="107"/>
-      <c r="B25" s="107"/>
-      <c r="C25" s="140" t="s">
+      <c r="A25" s="94"/>
+      <c r="B25" s="94"/>
+      <c r="C25" s="107" t="s">
         <v>9</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="E25" s="156" t="s">
+      <c r="E25" s="105" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="107"/>
-      <c r="B26" s="107"/>
-      <c r="C26" s="149"/>
+      <c r="A26" s="94"/>
+      <c r="B26" s="94"/>
+      <c r="C26" s="108"/>
       <c r="D26" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E26" s="157"/>
+      <c r="E26" s="106"/>
     </row>
     <row r="27" spans="1:5" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="107"/>
-      <c r="B27" s="107"/>
-      <c r="C27" s="149"/>
+      <c r="A27" s="94"/>
+      <c r="B27" s="94"/>
+      <c r="C27" s="108"/>
       <c r="D27" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="E27" s="156" t="s">
+      <c r="E27" s="105" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="107"/>
-      <c r="B28" s="107"/>
-      <c r="C28" s="141"/>
+      <c r="A28" s="94"/>
+      <c r="B28" s="94"/>
+      <c r="C28" s="109"/>
       <c r="D28" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E28" s="157"/>
+      <c r="E28" s="106"/>
     </row>
     <row r="29" spans="1:5" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="107"/>
-      <c r="B29" s="107"/>
+      <c r="A29" s="94"/>
+      <c r="B29" s="94"/>
       <c r="C29" s="7" t="s">
         <v>76</v>
       </c>
@@ -2886,8 +2900,8 @@
       </c>
     </row>
     <row r="30" spans="1:5" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="107"/>
-      <c r="B30" s="107"/>
+      <c r="A30" s="94"/>
+      <c r="B30" s="94"/>
       <c r="C30" s="36" t="s">
         <v>79</v>
       </c>
@@ -2897,9 +2911,9 @@
       </c>
     </row>
     <row r="31" spans="1:5" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="107"/>
-      <c r="B31" s="107"/>
-      <c r="C31" s="140" t="s">
+      <c r="A31" s="94"/>
+      <c r="B31" s="94"/>
+      <c r="C31" s="107" t="s">
         <v>10</v>
       </c>
       <c r="D31" s="6" t="s">
@@ -2910,9 +2924,9 @@
       </c>
     </row>
     <row r="32" spans="1:5" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="107"/>
-      <c r="B32" s="107"/>
-      <c r="C32" s="149"/>
+      <c r="A32" s="94"/>
+      <c r="B32" s="94"/>
+      <c r="C32" s="108"/>
       <c r="D32" s="6" t="s">
         <v>83</v>
       </c>
@@ -2921,9 +2935,9 @@
       </c>
     </row>
     <row r="33" spans="1:5" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="107"/>
-      <c r="B33" s="107"/>
-      <c r="C33" s="149"/>
+      <c r="A33" s="94"/>
+      <c r="B33" s="94"/>
+      <c r="C33" s="108"/>
       <c r="D33" s="6" t="s">
         <v>85</v>
       </c>
@@ -2932,9 +2946,9 @@
       </c>
     </row>
     <row r="34" spans="1:5" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="107"/>
-      <c r="B34" s="107"/>
-      <c r="C34" s="141"/>
+      <c r="A34" s="94"/>
+      <c r="B34" s="94"/>
+      <c r="C34" s="109"/>
       <c r="D34" s="6" t="s">
         <v>87</v>
       </c>
@@ -2943,8 +2957,8 @@
       </c>
     </row>
     <row r="35" spans="1:5" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="107"/>
-      <c r="B35" s="107"/>
+      <c r="A35" s="94"/>
+      <c r="B35" s="94"/>
       <c r="C35" s="7" t="s">
         <v>89</v>
       </c>
@@ -2954,8 +2968,8 @@
       </c>
     </row>
     <row r="36" spans="1:5" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="107"/>
-      <c r="B36" s="107"/>
+      <c r="A36" s="94"/>
+      <c r="B36" s="94"/>
       <c r="C36" s="7" t="s">
         <v>91</v>
       </c>
@@ -2967,8 +2981,8 @@
       </c>
     </row>
     <row r="37" spans="1:5" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="107"/>
-      <c r="B37" s="107"/>
+      <c r="A37" s="94"/>
+      <c r="B37" s="94"/>
       <c r="C37" s="36" t="s">
         <v>94</v>
       </c>
@@ -2978,10 +2992,10 @@
       </c>
     </row>
     <row r="38" spans="1:5" s="19" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="153">
+      <c r="A38" s="102">
         <v>4</v>
       </c>
-      <c r="B38" s="153" t="s">
+      <c r="B38" s="102" t="s">
         <v>11</v>
       </c>
       <c r="C38" s="43" t="s">
@@ -2995,9 +3009,9 @@
       </c>
     </row>
     <row r="39" spans="1:5" s="19" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="154"/>
-      <c r="B39" s="154"/>
-      <c r="C39" s="121" t="s">
+      <c r="A39" s="103"/>
+      <c r="B39" s="103"/>
+      <c r="C39" s="90" t="s">
         <v>98</v>
       </c>
       <c r="D39" s="17" t="s">
@@ -3008,9 +3022,9 @@
       </c>
     </row>
     <row r="40" spans="1:5" s="19" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="154"/>
-      <c r="B40" s="154"/>
-      <c r="C40" s="122"/>
+      <c r="A40" s="103"/>
+      <c r="B40" s="103"/>
+      <c r="C40" s="91"/>
       <c r="D40" s="42" t="s">
         <v>101</v>
       </c>
@@ -3019,9 +3033,9 @@
       </c>
     </row>
     <row r="41" spans="1:5" s="19" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="154"/>
-      <c r="B41" s="154"/>
-      <c r="C41" s="123"/>
+      <c r="A41" s="103"/>
+      <c r="B41" s="103"/>
+      <c r="C41" s="92"/>
       <c r="D41" s="42" t="s">
         <v>103</v>
       </c>
@@ -3030,8 +3044,8 @@
       </c>
     </row>
     <row r="42" spans="1:5" s="19" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="154"/>
-      <c r="B42" s="154"/>
+      <c r="A42" s="103"/>
+      <c r="B42" s="103"/>
       <c r="C42" s="20" t="s">
         <v>105</v>
       </c>
@@ -3041,9 +3055,9 @@
       </c>
     </row>
     <row r="43" spans="1:5" s="19" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="154"/>
-      <c r="B43" s="154"/>
-      <c r="C43" s="150" t="s">
+      <c r="A43" s="103"/>
+      <c r="B43" s="103"/>
+      <c r="C43" s="99" t="s">
         <v>107</v>
       </c>
       <c r="D43" s="30" t="s">
@@ -3054,9 +3068,9 @@
       </c>
     </row>
     <row r="44" spans="1:5" s="19" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="154"/>
-      <c r="B44" s="154"/>
-      <c r="C44" s="152"/>
+      <c r="A44" s="103"/>
+      <c r="B44" s="103"/>
+      <c r="C44" s="101"/>
       <c r="D44" s="30" t="s">
         <v>110</v>
       </c>
@@ -3065,9 +3079,9 @@
       </c>
     </row>
     <row r="45" spans="1:5" s="19" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="154"/>
-      <c r="B45" s="154"/>
-      <c r="C45" s="150" t="s">
+      <c r="A45" s="103"/>
+      <c r="B45" s="103"/>
+      <c r="C45" s="99" t="s">
         <v>112</v>
       </c>
       <c r="D45" s="30" t="s">
@@ -3078,9 +3092,9 @@
       </c>
     </row>
     <row r="46" spans="1:5" s="19" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="154"/>
-      <c r="B46" s="154"/>
-      <c r="C46" s="151"/>
+      <c r="A46" s="103"/>
+      <c r="B46" s="103"/>
+      <c r="C46" s="100"/>
       <c r="D46" s="30" t="s">
         <v>116</v>
       </c>
@@ -3089,9 +3103,9 @@
       </c>
     </row>
     <row r="47" spans="1:5" s="19" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="154"/>
-      <c r="B47" s="154"/>
-      <c r="C47" s="151"/>
+      <c r="A47" s="103"/>
+      <c r="B47" s="103"/>
+      <c r="C47" s="100"/>
       <c r="D47" s="30" t="s">
         <v>118</v>
       </c>
@@ -3100,9 +3114,9 @@
       </c>
     </row>
     <row r="48" spans="1:5" s="19" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="154"/>
-      <c r="B48" s="154"/>
-      <c r="C48" s="152"/>
+      <c r="A48" s="103"/>
+      <c r="B48" s="103"/>
+      <c r="C48" s="101"/>
       <c r="D48" s="30" t="s">
         <v>120</v>
       </c>
@@ -3111,9 +3125,9 @@
       </c>
     </row>
     <row r="49" spans="1:5" s="19" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="154"/>
-      <c r="B49" s="154"/>
-      <c r="C49" s="150" t="s">
+      <c r="A49" s="103"/>
+      <c r="B49" s="103"/>
+      <c r="C49" s="99" t="s">
         <v>121</v>
       </c>
       <c r="D49" s="46" t="s">
@@ -3124,9 +3138,9 @@
       </c>
     </row>
     <row r="50" spans="1:5" s="19" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="154"/>
-      <c r="B50" s="154"/>
-      <c r="C50" s="152"/>
+      <c r="A50" s="103"/>
+      <c r="B50" s="103"/>
+      <c r="C50" s="101"/>
       <c r="D50" s="46" t="s">
         <v>124</v>
       </c>
@@ -3135,8 +3149,8 @@
       </c>
     </row>
     <row r="51" spans="1:5" s="19" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="154"/>
-      <c r="B51" s="154"/>
+      <c r="A51" s="103"/>
+      <c r="B51" s="103"/>
       <c r="C51" s="48" t="s">
         <v>126</v>
       </c>
@@ -3146,9 +3160,9 @@
       </c>
     </row>
     <row r="52" spans="1:5" s="19" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="154"/>
-      <c r="B52" s="154"/>
-      <c r="C52" s="150" t="s">
+      <c r="A52" s="103"/>
+      <c r="B52" s="103"/>
+      <c r="C52" s="99" t="s">
         <v>13</v>
       </c>
       <c r="D52" s="30" t="s">
@@ -3159,9 +3173,9 @@
       </c>
     </row>
     <row r="53" spans="1:5" s="19" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="154"/>
-      <c r="B53" s="154"/>
-      <c r="C53" s="151"/>
+      <c r="A53" s="103"/>
+      <c r="B53" s="103"/>
+      <c r="C53" s="100"/>
       <c r="D53" s="30" t="s">
         <v>130</v>
       </c>
@@ -3170,9 +3184,9 @@
       </c>
     </row>
     <row r="54" spans="1:5" s="19" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="154"/>
-      <c r="B54" s="154"/>
-      <c r="C54" s="151"/>
+      <c r="A54" s="103"/>
+      <c r="B54" s="103"/>
+      <c r="C54" s="100"/>
       <c r="D54" s="30" t="s">
         <v>132</v>
       </c>
@@ -3181,9 +3195,9 @@
       </c>
     </row>
     <row r="55" spans="1:5" s="19" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="154"/>
-      <c r="B55" s="154"/>
-      <c r="C55" s="151"/>
+      <c r="A55" s="103"/>
+      <c r="B55" s="103"/>
+      <c r="C55" s="100"/>
       <c r="D55" s="30" t="s">
         <v>134</v>
       </c>
@@ -3192,9 +3206,9 @@
       </c>
     </row>
     <row r="56" spans="1:5" s="19" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="154"/>
-      <c r="B56" s="154"/>
-      <c r="C56" s="151"/>
+      <c r="A56" s="103"/>
+      <c r="B56" s="103"/>
+      <c r="C56" s="100"/>
       <c r="D56" s="30" t="s">
         <v>136</v>
       </c>
@@ -3203,9 +3217,9 @@
       </c>
     </row>
     <row r="57" spans="1:5" s="19" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="154"/>
-      <c r="B57" s="154"/>
-      <c r="C57" s="152"/>
+      <c r="A57" s="103"/>
+      <c r="B57" s="103"/>
+      <c r="C57" s="101"/>
       <c r="D57" s="30" t="s">
         <v>138</v>
       </c>
@@ -3214,8 +3228,8 @@
       </c>
     </row>
     <row r="58" spans="1:5" s="19" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="154"/>
-      <c r="B58" s="154"/>
+      <c r="A58" s="103"/>
+      <c r="B58" s="103"/>
       <c r="C58" s="48" t="s">
         <v>140</v>
       </c>
@@ -3225,8 +3239,8 @@
       </c>
     </row>
     <row r="59" spans="1:5" s="19" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="154"/>
-      <c r="B59" s="154"/>
+      <c r="A59" s="103"/>
+      <c r="B59" s="103"/>
       <c r="C59" s="47" t="s">
         <v>142</v>
       </c>
@@ -3236,8 +3250,8 @@
       </c>
     </row>
     <row r="60" spans="1:5" s="19" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="155"/>
-      <c r="B60" s="155"/>
+      <c r="A60" s="104"/>
+      <c r="B60" s="104"/>
       <c r="C60" s="48" t="s">
         <v>144</v>
       </c>
@@ -3247,10 +3261,10 @@
       </c>
     </row>
     <row r="61" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="135">
+      <c r="A61" s="126">
         <v>6</v>
       </c>
-      <c r="B61" s="135" t="s">
+      <c r="B61" s="126" t="s">
         <v>14</v>
       </c>
       <c r="C61" s="26" t="s">
@@ -3262,8 +3276,8 @@
       </c>
     </row>
     <row r="62" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="136"/>
-      <c r="B62" s="136"/>
+      <c r="A62" s="127"/>
+      <c r="B62" s="127"/>
       <c r="C62" s="26" t="s">
         <v>148</v>
       </c>
@@ -3273,8 +3287,8 @@
       </c>
     </row>
     <row r="63" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="136"/>
-      <c r="B63" s="136"/>
+      <c r="A63" s="127"/>
+      <c r="B63" s="127"/>
       <c r="C63" s="26" t="s">
         <v>150</v>
       </c>
@@ -3286,8 +3300,8 @@
       </c>
     </row>
     <row r="64" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="136"/>
-      <c r="B64" s="136"/>
+      <c r="A64" s="127"/>
+      <c r="B64" s="127"/>
       <c r="C64" s="26" t="s">
         <v>154</v>
       </c>
@@ -3297,10 +3311,10 @@
       </c>
     </row>
     <row r="65" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="131">
+      <c r="A65" s="123">
         <v>7</v>
       </c>
-      <c r="B65" s="131" t="s">
+      <c r="B65" s="123" t="s">
         <v>15</v>
       </c>
       <c r="C65" s="21" t="s">
@@ -3312,8 +3326,8 @@
       </c>
     </row>
     <row r="66" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="132"/>
-      <c r="B66" s="132"/>
+      <c r="A66" s="124"/>
+      <c r="B66" s="124"/>
       <c r="C66" s="21" t="s">
         <v>157</v>
       </c>
@@ -3323,8 +3337,8 @@
       </c>
     </row>
     <row r="67" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="132"/>
-      <c r="B67" s="132"/>
+      <c r="A67" s="124"/>
+      <c r="B67" s="124"/>
       <c r="C67" s="21" t="s">
         <v>159</v>
       </c>
@@ -3334,8 +3348,8 @@
       </c>
     </row>
     <row r="68" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="132"/>
-      <c r="B68" s="132"/>
+      <c r="A68" s="124"/>
+      <c r="B68" s="124"/>
       <c r="C68" s="21" t="s">
         <v>161</v>
       </c>
@@ -3345,8 +3359,8 @@
       </c>
     </row>
     <row r="69" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="132"/>
-      <c r="B69" s="132"/>
+      <c r="A69" s="124"/>
+      <c r="B69" s="124"/>
       <c r="C69" s="21" t="s">
         <v>162</v>
       </c>
@@ -3358,8 +3372,8 @@
       </c>
     </row>
     <row r="70" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="132"/>
-      <c r="B70" s="132"/>
+      <c r="A70" s="124"/>
+      <c r="B70" s="124"/>
       <c r="C70" s="21" t="s">
         <v>165</v>
       </c>
@@ -3369,46 +3383,46 @@
       </c>
     </row>
     <row r="71" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="132"/>
-      <c r="B71" s="132"/>
+      <c r="A71" s="124"/>
+      <c r="B71" s="124"/>
       <c r="C71" s="21" t="s">
         <v>166</v>
       </c>
       <c r="D71" s="22"/>
-      <c r="E71" s="127" t="s">
+      <c r="E71" s="120" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="72" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="132"/>
-      <c r="B72" s="132"/>
+      <c r="A72" s="124"/>
+      <c r="B72" s="124"/>
       <c r="C72" s="21" t="s">
         <v>168</v>
       </c>
       <c r="D72" s="22"/>
-      <c r="E72" s="134"/>
+      <c r="E72" s="121"/>
     </row>
     <row r="73" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="132"/>
-      <c r="B73" s="132"/>
+      <c r="A73" s="124"/>
+      <c r="B73" s="124"/>
       <c r="C73" s="21" t="s">
         <v>169</v>
       </c>
       <c r="D73" s="22"/>
-      <c r="E73" s="134"/>
+      <c r="E73" s="121"/>
     </row>
     <row r="74" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="132"/>
-      <c r="B74" s="132"/>
+      <c r="A74" s="124"/>
+      <c r="B74" s="124"/>
       <c r="C74" s="21" t="s">
         <v>170</v>
       </c>
       <c r="D74" s="22"/>
-      <c r="E74" s="128"/>
+      <c r="E74" s="122"/>
     </row>
     <row r="75" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="132"/>
-      <c r="B75" s="132"/>
+      <c r="A75" s="124"/>
+      <c r="B75" s="124"/>
       <c r="C75" s="21" t="s">
         <v>171</v>
       </c>
@@ -3418,30 +3432,30 @@
       </c>
     </row>
     <row r="76" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="132"/>
-      <c r="B76" s="132"/>
+      <c r="A76" s="124"/>
+      <c r="B76" s="124"/>
       <c r="C76" s="21" t="s">
         <v>173</v>
       </c>
       <c r="D76" s="22"/>
-      <c r="E76" s="127" t="s">
+      <c r="E76" s="120" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="77" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="133"/>
-      <c r="B77" s="133"/>
+      <c r="A77" s="125"/>
+      <c r="B77" s="125"/>
       <c r="C77" s="21" t="s">
         <v>175</v>
       </c>
       <c r="D77" s="22"/>
-      <c r="E77" s="128"/>
+      <c r="E77" s="122"/>
     </row>
     <row r="78" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="131">
+      <c r="A78" s="123">
         <v>8</v>
       </c>
-      <c r="B78" s="131" t="s">
+      <c r="B78" s="123" t="s">
         <v>16</v>
       </c>
       <c r="C78" s="21" t="s">
@@ -3453,8 +3467,8 @@
       </c>
     </row>
     <row r="79" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="132"/>
-      <c r="B79" s="132"/>
+      <c r="A79" s="124"/>
+      <c r="B79" s="124"/>
       <c r="C79" s="54" t="s">
         <v>178</v>
       </c>
@@ -3464,28 +3478,28 @@
       </c>
     </row>
     <row r="80" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="132"/>
-      <c r="B80" s="132"/>
+      <c r="A80" s="124"/>
+      <c r="B80" s="124"/>
       <c r="C80" s="21" t="s">
         <v>180</v>
       </c>
       <c r="D80" s="22"/>
-      <c r="E80" s="127" t="s">
+      <c r="E80" s="120" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="81" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="132"/>
-      <c r="B81" s="132"/>
+      <c r="A81" s="124"/>
+      <c r="B81" s="124"/>
       <c r="C81" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D81" s="22"/>
-      <c r="E81" s="128"/>
+      <c r="E81" s="122"/>
     </row>
     <row r="82" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="132"/>
-      <c r="B82" s="132"/>
+      <c r="A82" s="124"/>
+      <c r="B82" s="124"/>
       <c r="C82" s="21" t="s">
         <v>183</v>
       </c>
@@ -3495,8 +3509,8 @@
       </c>
     </row>
     <row r="83" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="132"/>
-      <c r="B83" s="132"/>
+      <c r="A83" s="124"/>
+      <c r="B83" s="124"/>
       <c r="C83" s="21" t="s">
         <v>185</v>
       </c>
@@ -3506,8 +3520,8 @@
       </c>
     </row>
     <row r="84" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="132"/>
-      <c r="B84" s="132"/>
+      <c r="A84" s="124"/>
+      <c r="B84" s="124"/>
       <c r="C84" s="21" t="s">
         <v>187</v>
       </c>
@@ -3517,8 +3531,8 @@
       </c>
     </row>
     <row r="85" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="132"/>
-      <c r="B85" s="132"/>
+      <c r="A85" s="124"/>
+      <c r="B85" s="124"/>
       <c r="C85" s="21" t="s">
         <v>189</v>
       </c>
@@ -3528,48 +3542,48 @@
       </c>
     </row>
     <row r="86" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="132"/>
-      <c r="B86" s="132"/>
+      <c r="A86" s="124"/>
+      <c r="B86" s="124"/>
       <c r="C86" s="21" t="s">
         <v>191</v>
       </c>
       <c r="D86" s="22"/>
-      <c r="E86" s="127" t="s">
+      <c r="E86" s="120" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="87" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="132"/>
-      <c r="B87" s="132"/>
+      <c r="A87" s="124"/>
+      <c r="B87" s="124"/>
       <c r="C87" s="21" t="s">
         <v>193</v>
       </c>
       <c r="D87" s="22"/>
-      <c r="E87" s="128"/>
+      <c r="E87" s="122"/>
     </row>
     <row r="88" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="132"/>
-      <c r="B88" s="132"/>
+      <c r="A88" s="124"/>
+      <c r="B88" s="124"/>
       <c r="C88" s="21" t="s">
         <v>194</v>
       </c>
       <c r="D88" s="22"/>
-      <c r="E88" s="129" t="s">
+      <c r="E88" s="131" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="89" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="132"/>
-      <c r="B89" s="132"/>
+      <c r="A89" s="124"/>
+      <c r="B89" s="124"/>
       <c r="C89" s="21" t="s">
         <v>196</v>
       </c>
       <c r="D89" s="22"/>
-      <c r="E89" s="130"/>
+      <c r="E89" s="132"/>
     </row>
     <row r="90" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="132"/>
-      <c r="B90" s="132"/>
+      <c r="A90" s="124"/>
+      <c r="B90" s="124"/>
       <c r="C90" s="21" t="s">
         <v>197</v>
       </c>
@@ -3579,8 +3593,8 @@
       </c>
     </row>
     <row r="91" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="132"/>
-      <c r="B91" s="132"/>
+      <c r="A91" s="124"/>
+      <c r="B91" s="124"/>
       <c r="C91" s="21" t="s">
         <v>199</v>
       </c>
@@ -3590,8 +3604,8 @@
       </c>
     </row>
     <row r="92" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="133"/>
-      <c r="B92" s="133"/>
+      <c r="A92" s="125"/>
+      <c r="B92" s="125"/>
       <c r="C92" s="21" t="s">
         <v>201</v>
       </c>
@@ -3601,45 +3615,45 @@
       </c>
     </row>
     <row r="93" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="124">
+      <c r="A93" s="128">
         <v>9</v>
       </c>
-      <c r="B93" s="124" t="s">
+      <c r="B93" s="128" t="s">
         <v>17</v>
       </c>
       <c r="C93" s="13" t="s">
         <v>203</v>
       </c>
       <c r="D93" s="25"/>
-      <c r="E93" s="59" t="s">
+      <c r="E93" s="57" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="94" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="125"/>
-      <c r="B94" s="125"/>
+      <c r="A94" s="129"/>
+      <c r="B94" s="129"/>
       <c r="C94" s="13" t="s">
         <v>204</v>
       </c>
       <c r="D94" s="25"/>
-      <c r="E94" s="60" t="s">
+      <c r="E94" s="58" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="95" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="125"/>
-      <c r="B95" s="125"/>
+      <c r="A95" s="129"/>
+      <c r="B95" s="129"/>
       <c r="C95" s="13" t="s">
         <v>205</v>
       </c>
       <c r="D95" s="25"/>
-      <c r="E95" s="58" t="s">
+      <c r="E95" s="56" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="96" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="125"/>
-      <c r="B96" s="125"/>
+      <c r="A96" s="129"/>
+      <c r="B96" s="129"/>
       <c r="C96" s="55" t="s">
         <v>206</v>
       </c>
@@ -3649,8 +3663,8 @@
       </c>
     </row>
     <row r="97" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="125"/>
-      <c r="B97" s="125"/>
+      <c r="A97" s="129"/>
+      <c r="B97" s="129"/>
       <c r="C97" s="55" t="s">
         <v>211</v>
       </c>
@@ -3662,8 +3676,8 @@
       </c>
     </row>
     <row r="98" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="125"/>
-      <c r="B98" s="125"/>
+      <c r="A98" s="129"/>
+      <c r="B98" s="129"/>
       <c r="C98" s="55" t="s">
         <v>214</v>
       </c>
@@ -3673,8 +3687,8 @@
       </c>
     </row>
     <row r="99" spans="1:5" s="15" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="126"/>
-      <c r="B99" s="126"/>
+      <c r="A99" s="130"/>
+      <c r="B99" s="130"/>
       <c r="C99" s="13" t="s">
         <v>216</v>
       </c>
@@ -3888,6 +3902,31 @@
     <row r="162" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="B93:B99"/>
+    <mergeCell ref="A93:A99"/>
+    <mergeCell ref="E80:E81"/>
+    <mergeCell ref="E86:E87"/>
+    <mergeCell ref="E88:E89"/>
+    <mergeCell ref="B78:B92"/>
+    <mergeCell ref="A78:A92"/>
+    <mergeCell ref="E71:E74"/>
+    <mergeCell ref="B65:B77"/>
+    <mergeCell ref="A65:A77"/>
+    <mergeCell ref="E76:E77"/>
+    <mergeCell ref="B61:B64"/>
+    <mergeCell ref="A61:A64"/>
+    <mergeCell ref="B2:B11"/>
+    <mergeCell ref="A2:A11"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="A12:A17"/>
+    <mergeCell ref="B12:B17"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="E13:E16"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="C21:C22"/>
     <mergeCell ref="C52:C57"/>
     <mergeCell ref="B38:B60"/>
     <mergeCell ref="A38:A60"/>
@@ -3901,31 +3940,6 @@
     <mergeCell ref="A18:A37"/>
     <mergeCell ref="B18:B37"/>
     <mergeCell ref="C49:C50"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="E13:E16"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="B2:B11"/>
-    <mergeCell ref="A2:A11"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A12:A17"/>
-    <mergeCell ref="B12:B17"/>
-    <mergeCell ref="E71:E74"/>
-    <mergeCell ref="B65:B77"/>
-    <mergeCell ref="A65:A77"/>
-    <mergeCell ref="E76:E77"/>
-    <mergeCell ref="B61:B64"/>
-    <mergeCell ref="A61:A64"/>
-    <mergeCell ref="B93:B99"/>
-    <mergeCell ref="A93:A99"/>
-    <mergeCell ref="E80:E81"/>
-    <mergeCell ref="E86:E87"/>
-    <mergeCell ref="E88:E89"/>
-    <mergeCell ref="B78:B92"/>
-    <mergeCell ref="A78:A92"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>